<commit_message>
problematique.md : new file, and gestion_projet updated. Clementine's try of modelisation (class diagramof actors).
</commit_message>
<xml_diff>
--- a/Documentation/Documents-Liens-Bibliographie.xlsx
+++ b/Documentation/Documents-Liens-Bibliographie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="250" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>LISTE DES LIENS INTERESSANTS POUR LE PROJET MODELISATION ET STRUCTURATION D'UN SI</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>http://www.vignevin.com</t>
+  </si>
+  <si>
+    <t>Food info</t>
+  </si>
+  <si>
+    <t>http://www.food-info.net/fr/products/wine/prod.htm</t>
+  </si>
+  <si>
+    <t>observatoire de la viticulture française</t>
+  </si>
+  <si>
+    <t>http://www.observatoire-viti-france.com</t>
+  </si>
+  <si>
+    <t>Logiciel de gestion viti_vinicole</t>
+  </si>
+  <si>
+    <t>Lavilog</t>
+  </si>
+  <si>
+    <t>http://www.lavilog.com</t>
   </si>
 </sst>
 </file>
@@ -78,7 +99,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -122,12 +143,6 @@
       <color rgb="000563C1"/>
       <sz val="12"/>
       <u val="single"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +162,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -171,18 +186,14 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -190,16 +201,14 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="15"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -269,18 +278,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
+      <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.8745098039216"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4980392156863"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.5372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.4980392156863"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.9137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="1">
@@ -333,7 +342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="5">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -351,11 +360,44 @@
       <c r="A6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -364,6 +406,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink display="https://www.youtube.com/watch?v=nlQnOWr9gpc" ref="D4" r:id="rId1"/>
+    <hyperlink display="http://www.food-info.net/fr/products/wine/prod.htm" ref="D7" r:id="rId2"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>